<commit_message>
Added create text feauture
</commit_message>
<xml_diff>
--- a/WZ_BACKEND/Design Tool/API.xlsx
+++ b/WZ_BACKEND/Design Tool/API.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>None</t>
   </si>
@@ -137,9 +137,6 @@
     </r>
   </si>
   <si>
-    <t>DisplayState(int id)</t>
-  </si>
-  <si>
     <t>Tells the editor to display to change the state to the specified id</t>
   </si>
   <si>
@@ -166,6 +163,15 @@
     </r>
   </si>
   <si>
+    <t>ChangeStateName(string arg)</t>
+  </si>
+  <si>
+    <t>createState(id,name)</t>
+  </si>
+  <si>
+    <t>DisplayState()</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -185,14 +191,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> :SendMessage ('Facade', 'DisplayState',1);</t>
-    </r>
-  </si>
-  <si>
-    <t>Tells the editor to change the name of the specified state. Requires you to pass a string and seprate arguments with a comma</t>
-  </si>
-  <si>
-    <t>ChangeStateName(string arg)</t>
+      <t xml:space="preserve">:SendMessage('Façade','ChangeStateName','this is a new name'); </t>
+    </r>
+  </si>
+  <si>
+    <t>Tells the editor to change the name of the target state. Requires you to pass a string and seprate arguments with a comma</t>
+  </si>
+  <si>
+    <t>DeleteState()</t>
   </si>
   <si>
     <r>
@@ -214,11 +220,66 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>:SendMessage('Façade','ChangeStateName',arg);  var arr =  "1,this is a new name"</t>
-    </r>
-  </si>
-  <si>
-    <t>createState(id,name)</t>
+      <t xml:space="preserve"> :SendMessage ('Facade', 'DeleteState');</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :SendMessage ('Facade', 'DisplayState');</t>
+    </r>
+  </si>
+  <si>
+    <t>SetTargetState(int id)</t>
+  </si>
+  <si>
+    <t>Operations that target states would be targetting the specified state from now on</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SendMessage ('Facade', SetTargetState',id);</t>
+    </r>
+  </si>
+  <si>
+    <t>SetTargetStateObject(int id)</t>
+  </si>
+  <si>
+    <t>Operations that target states would be targetting the specified state object from now on</t>
   </si>
 </sst>
 </file>
@@ -623,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +766,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
@@ -725,7 +786,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -740,7 +801,7 @@
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -748,19 +809,19 @@
         <v>0</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,23 +829,86 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>

</xml_diff>